<commit_message>
Atualização automática de LAVRAS_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/LAVRAS_DO_SUL.xlsx
+++ b/LAVRAS_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0308CF6-39CE-4718-B386-938AC1727B34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C106BD2E-A9B6-4D3A-9834-E6F9E5F169AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,20 +20,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="4" r:id="rId5"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="5" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1019,7 +1006,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1079,36 +1066,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1142,14 +1105,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1166,7 +1125,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1199,7 +1157,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{10B6AEC7-EF9F-403B-98AE-47F943089876}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{D5DF0B5F-E90C-42F0-91A7-1B75A08920F8}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1229,10 +1187,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{80FBF315-BFB1-4E88-853B-514E94D7C4A1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CDB6D5D-97E0-44F8-A647-92C950749D29}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1270,7 +1228,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB99CB06-4B85-4A30-807A-D6F77B56E502}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{33704DF4-D923-47AD-B7BE-F1BF821F6A31}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1333,7 +1291,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ACBCB66-9DA8-40C6-BFA0-9FE6EDD69E1C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89F67FD7-E6E2-424D-AD69-372086630A28}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1352,7 +1310,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{752CB487-6C6B-5680-D943-F9EDB483C1F4}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EB17A57-D761-DBD2-1A52-22CBAA9AF1A2}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1401,7 +1359,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05143323-4239-04C4-ACDD-01466B6A1A66}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BAC20A2-DA66-EAFB-6914-BF36E28B35E6}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1420,7 +1378,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5764EA85-7C59-7050-3079-A2F9781F089B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F88D905-D88C-9B2E-F0AC-FB6C25F2A750}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1451,7 +1409,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D043C545-15FC-992E-7ACA-F765393E5A37}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A8AED3E4-8D95-CE8A-2289-5932E43302E6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1482,7 +1440,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9C69FD0-3F22-D108-24CE-F3A5DA675FED}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3793291C-BD3F-D889-7BE0-E9DEF226CBAB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1525,7 +1483,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E75619F1-FD46-4F67-91E0-BE958A3CACC2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0696D294-15AD-4172-B5B3-DF754B1774AC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1563,7 +1521,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFAFD17B-176D-4674-A889-E832556D1238}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE66E8DE-7A6F-454F-9424-FBE599DF914B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1606,7 +1564,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F14361C0-68B9-40B6-B114-5A8E7B2C7D4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4C84FA6-4E49-4441-9BB2-362137A8C7DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1919,7 +1877,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3F0A09C-51D4-4F78-A4CB-66EEC26A2350}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D82E4B71-4096-4328-870F-1F6F8B8B80F7}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -1931,98 +1889,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="36"/>
-    <col min="6" max="6" width="2" style="36" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="36"/>
+    <col min="1" max="5" width="12.5703125" style="33"/>
+    <col min="6" max="6" width="2" style="33" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="33" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="35"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="35"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="35"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="35"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="35"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="35"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="35"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="35"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="35"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="35"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="35"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="35"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="35"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="35"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="35"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="35"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="35"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="35"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="35"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="35"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="35"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="35"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="35"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="35"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="35"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="35"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="35"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="35"/>
+      <c r="F29" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5169,19 +5127,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="13" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>256</v>
       </c>
     </row>
@@ -5204,46 +5162,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="15" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="15" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="17" t="s">
         <v>259</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="17" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="17" t="s">
         <v>261</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="17" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="17" t="s">
         <v>260</v>
       </c>
     </row>
@@ -5268,99 +5226,100 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="18" t="s">
         <v>264</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="19" t="s">
         <v>265</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="19" t="s">
         <v>267</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="19" t="s">
         <v>268</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="20" t="s">
         <v>269</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="20" t="s">
         <v>270</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="I1" s="20" t="s">
+      <c r="I1" s="18" t="s">
         <v>272</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="18" t="s">
         <v>273</v>
       </c>
-      <c r="K1" s="20" t="s">
+      <c r="K1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="L1" s="20" t="s">
+      <c r="L1" s="18" t="s">
         <v>275</v>
       </c>
-      <c r="M1" s="20" t="s">
+      <c r="M1" s="18" t="s">
         <v>276</v>
       </c>
-      <c r="N1" s="20" t="s">
+      <c r="N1" s="18" t="s">
         <v>277</v>
       </c>
-      <c r="O1" s="20" t="s">
+      <c r="O1" s="18" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="14" t="s">
         <v>279</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="21">
         <v>45839</v>
       </c>
-      <c r="D2" s="25"/>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="F2" s="26">
+      <c r="F2" s="23">
         <v>2478</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="23">
         <v>374</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="K2" s="27" t="s">
+      <c r="K2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="L2" s="27" t="s">
+      <c r="L2" s="24" t="s">
         <v>281</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="25" t="s">
         <v>283</v>
       </c>
-      <c r="N2" s="23" t="s">
+      <c r="N2" s="14" t="s">
         <v>282</v>
       </c>
-      <c r="O2" s="28" t="s">
+      <c r="O2" s="25" t="s">
         <v>283</v>
       </c>
     </row>
@@ -5385,31 +5344,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="26" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="26" t="s">
         <v>284</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="27" t="s">
         <v>285</v>
       </c>
-      <c r="E1" s="31">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="28">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="29">
         <v>1</v>
       </c>
-      <c r="F1" s="32">
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="31">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="33" t="s">
-        <v>286</v>
-      </c>
-      <c r="B2" s="34">
-        <v>1</v>
-      </c>
-      <c r="C2" s="32">
+      <c r="C2" s="29">
         <v>6.612881893929374E-5</v>
       </c>
     </row>

</xml_diff>